<commit_message>
Final result:- MAPE: 2.79% RMSE: 13434.94 KW
</commit_message>
<xml_diff>
--- a/model_testing.xlsx
+++ b/model_testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SDUST-Masters\Code\asgn1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAE0525-3337-42B5-9B4E-1AEC5B596FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89F21F9-0B4C-4D23-A22C-75B6CD3AB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0759573-7E7B-477A-ADB4-F1461526A75A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>max_norm</t>
   </si>
@@ -68,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -150,7 +150,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -503,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D4CC93-0070-4FA3-84AC-76CDEFF991F9}">
-  <dimension ref="C2:O28"/>
+  <dimension ref="C2:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -522,10 +522,15 @@
     <col min="13" max="13" width="12" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.88671875" style="2" customWidth="1"/>
     <col min="15" max="15" width="13.5546875" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="1"/>
+    <col min="16" max="16" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" style="1"/>
+    <col min="20" max="20" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
@@ -559,8 +564,20 @@
       <c r="O2" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -594,8 +611,20 @@
       <c r="O3" s="5">
         <v>36366.557699999998</v>
       </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q3" s="2">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2">
+        <v>32</v>
+      </c>
+      <c r="S3" s="4">
+        <v>4.2410000000000003E-2</v>
+      </c>
+      <c r="T3" s="5">
+        <v>25007.495900000002</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -629,8 +658,12 @@
       <c r="O4" s="5">
         <v>25364.5389</v>
       </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C5" s="2">
         <v>3</v>
       </c>
@@ -664,8 +697,12 @@
       <c r="O5" s="5">
         <v>27089.4653</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C6" s="2">
         <v>4</v>
       </c>
@@ -699,8 +736,12 @@
       <c r="O6" s="5">
         <v>24829.2238</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C7" s="2">
         <v>5</v>
       </c>
@@ -734,8 +775,12 @@
       <c r="O7" s="8">
         <v>24303.840499999998</v>
       </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="15"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C8" s="2">
         <v>6</v>
       </c>
@@ -769,8 +814,12 @@
       <c r="O8" s="5">
         <v>24436.8024</v>
       </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="15"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C9" s="6">
         <v>7</v>
       </c>
@@ -804,8 +853,12 @@
       <c r="O9" s="8">
         <v>24596.8429</v>
       </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="15"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -839,8 +892,12 @@
       <c r="O10" s="5">
         <v>25071.122599999999</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="15"/>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <v>9</v>
       </c>
@@ -874,8 +931,12 @@
       <c r="O11" s="5">
         <v>25025.730200000002</v>
       </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>10</v>
       </c>
@@ -909,14 +970,18 @@
       <c r="O12" s="5">
         <v>26836.628100000002</v>
       </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="15"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D15" s="3"/>
       <c r="H15" s="11" t="s">
         <v>3</v>
@@ -943,7 +1008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:20" x14ac:dyDescent="0.3">
       <c r="D16" s="3"/>
       <c r="H16" s="2">
         <v>50</v>
@@ -960,7 +1025,7 @@
       <c r="L16" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N16" s="4">
@@ -987,7 +1052,7 @@
       <c r="L17" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N17" s="4">
@@ -1040,13 +1105,13 @@
       <c r="L19" s="2">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="M19" s="13">
+      <c r="M19" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N19" s="4">
         <v>4.2356999999999999E-2</v>
       </c>
-      <c r="O19" s="15">
+      <c r="O19" s="5">
         <v>24976.132699999998</v>
       </c>
     </row>
@@ -1066,7 +1131,7 @@
       <c r="L20" s="2">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N20" s="4">
@@ -1077,28 +1142,28 @@
       </c>
     </row>
     <row r="21" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="H21" s="13">
-        <v>50</v>
-      </c>
-      <c r="I21" s="13">
-        <v>32</v>
-      </c>
-      <c r="J21" s="13">
-        <v>4</v>
-      </c>
-      <c r="K21" s="13">
-        <v>64</v>
-      </c>
-      <c r="L21" s="13">
+      <c r="H21" s="2">
+        <v>50</v>
+      </c>
+      <c r="I21" s="2">
+        <v>32</v>
+      </c>
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>64</v>
+      </c>
+      <c r="L21" s="2">
         <v>0.01</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="N21" s="14">
+      <c r="N21" s="4">
         <v>4.3535999999999998E-2</v>
       </c>
-      <c r="O21" s="15">
+      <c r="O21" s="5">
         <v>25589.2592</v>
       </c>
     </row>
@@ -1118,7 +1183,7 @@
       <c r="L22" s="2">
         <v>0.1</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="N22" s="4">
@@ -1134,7 +1199,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="13"/>
+      <c r="M27" s="2"/>
       <c r="N27" s="4"/>
       <c r="O27" s="5"/>
     </row>
@@ -1144,7 +1209,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="13"/>
+      <c r="M28" s="2"/>
       <c r="N28" s="4"/>
       <c r="O28" s="5"/>
     </row>

</xml_diff>